<commit_message>
fix(IP's): corregir ips por nuevo enunciado
- Lado derecho tienen 3 redes nuevas debido a modificacion: por lo que se agregaron 3 nuevas gateways y las pc se le asignaron nueva ip. Modificado en la tabla de excel
</commit_message>
<xml_diff>
--- a/Practica1/IP/Subneting.xlsx
+++ b/Practica1/IP/Subneting.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\GitKraken\REDES2_1S2025_G37\IP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ingenieriausacedu-my.sharepoint.com/personal/201903549_ingenieria_usac_edu_gt/Documents/13_1s24/975 lab/Pra/1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8F3BB1-CEF0-42D9-9B89-E060BF626FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{5E8F3BB1-CEF0-42D9-9B89-E060BF626FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99BB58DD-5119-4686-A9DE-2FD6C2C9D8BA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7FB8CBF1-6F7F-4229-BDCA-ACC21E0E5DCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{7FB8CBF1-6F7F-4229-BDCA-ACC21E0E5DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="VLSM" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="68">
   <si>
     <t>Dispositivo</t>
   </si>
@@ -210,22 +210,37 @@
     <t>192.168.11.4</t>
   </si>
   <si>
-    <t>192.168.11.5</t>
-  </si>
-  <si>
-    <t>192.168.11.6</t>
-  </si>
-  <si>
     <t>192.168.21.3</t>
   </si>
   <si>
-    <t>192.168.21.4</t>
-  </si>
-  <si>
     <t>192.168.31.4</t>
   </si>
   <si>
     <t>Asignar ips sin vlsm</t>
+  </si>
+  <si>
+    <t>192.168.41.1</t>
+  </si>
+  <si>
+    <t>192.168.51.1</t>
+  </si>
+  <si>
+    <t>192.168.61.1</t>
+  </si>
+  <si>
+    <t>192.168.41.2</t>
+  </si>
+  <si>
+    <t>192.168.61.2</t>
+  </si>
+  <si>
+    <t>192.168.51.2</t>
+  </si>
+  <si>
+    <t>192.168.41.3</t>
+  </si>
+  <si>
+    <t>192.168.51.3</t>
   </si>
 </sst>
 </file>
@@ -263,7 +278,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -309,6 +324,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -377,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -403,6 +424,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -745,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E01EA280-285F-4E3D-A99F-76398A9CB501}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A6" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1196,8 +1220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C291CB1C-C965-481E-B8AB-A2977D7D8D28}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1214,7 +1238,7 @@
         <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
         <v>54</v>
@@ -1367,7 +1391,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="18" t="s">
         <v>33</v>
       </c>
       <c r="B13" s="15" t="s">
@@ -1377,7 +1401,7 @@
         <v>24</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>55</v>
@@ -1392,7 +1416,7 @@
         <v>25</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>55</v>
@@ -1407,7 +1431,7 @@
         <v>26</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>55</v>
@@ -1472,7 +1496,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="18" t="s">
         <v>33</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -1482,13 +1506,13 @@
         <v>4</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>55</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1522,7 +1546,7 @@
         <v>4</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>55</v>
@@ -1532,7 +1556,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="18" t="s">
         <v>33</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -1542,17 +1566,17 @@
         <v>4</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>55</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="18" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1562,17 +1586,17 @@
         <v>4</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>55</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="18" t="s">
         <v>33</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -1582,13 +1606,13 @@
         <v>4</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>55</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1602,7 +1626,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>55</v>
@@ -1612,7 +1636,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="18" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="6" t="s">
@@ -1622,13 +1646,13 @@
         <v>4</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>55</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>